<commit_message>
ETB and HTB updates locates with shortsell Order
</commit_message>
<xml_diff>
--- a/src/test/java/LocatesAPI/Data/Locates.xlsx
+++ b/src/test/java/LocatesAPI/Data/Locates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_OMSAPI\src\test\java\LocatesAPI\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AA3D2E-9F8E-4900-B2B1-22BE6562F7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241711E5-65BD-4775-9936-EEA194AD4975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="664" activeTab="3" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Locates" sheetId="33" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="185">
   <si>
     <t>Content_Type</t>
   </si>
@@ -581,6 +581,94 @@
   </si>
   <si>
     <t>1LOC-LOCA-123456-M_AAA</t>
+  </si>
+  <si>
+    <t>/int/ord/api/V3/orders</t>
+  </si>
+  <si>
+    <t>Order successfully created.</t>
+  </si>
+  <si>
+    <t>ShortSell_Order_Creation_BasePath</t>
+  </si>
+  <si>
+    <t>ShortSell_Order_Creation_Body</t>
+  </si>
+  <si>
+    <t>ShortSell_Order_Creation_StatusCode</t>
+  </si>
+  <si>
+    <t>ShortSell_Order_Creation_Response</t>
+  </si>
+  <si>
+    <t>{
+    "ordType": "2",
+    "side": "5",
+    "timeInForce": "0",
+    "destination": "D0",
+    "account": "1LOC-LOCA-123456-M",
+    "orderQty":100,
+    "symbol": "MSFT",
+    "Price": 70,
+    "StopPx": 0
+ }</t>
+  </si>
+  <si>
+    <t>{
+    "ordType": "2",
+    "side": "5",
+    "timeInForce": "0",
+    "destination": "D0",
+    "account": "1LOC-LOCA-123456-M",
+    "orderQty":200,
+    "symbol": "IBM",
+    "Price": 70,
+    "StopPx": 0
+ }</t>
+  </si>
+  <si>
+    <t>{
+    "ordType": "2",
+    "side": "5",
+    "timeInForce": "0",
+    "destination": "D0",
+    "account": "1LOC-LOCA-123456-M",
+    "orderQty":300,
+    "symbol": "A",
+    "Price": 70,
+    "StopPx": 0
+ }</t>
+  </si>
+  <si>
+    <t>{
+    "ordType": "2",
+    "side": "5",
+    "timeInForce": "0",
+    "destination": "D0",
+    "account": "1LOC-LOCA-123456-M",
+    "orderQty":400,
+    "symbol": "AA",
+    "Price": 70,
+    "StopPx": 0
+ }</t>
+  </si>
+  <si>
+    <t>ShortSell_Order_Quantity</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>HTB_Flag</t>
+  </si>
+  <si>
+    <t>EndpointVersion</t>
+  </si>
+  <si>
+    <t>V3</t>
   </si>
 </sst>
 </file>
@@ -652,7 +740,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -675,6 +763,11 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A8C1AD-EA4E-465E-9419-F066525F9C3B}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2756,1251 +2849,1363 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E145D5-C6BB-45CB-9B3A-6509F3104821}">
-  <dimension ref="A1:BZ5"/>
+  <dimension ref="A1:CG5"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="3" customWidth="1"/>
-    <col min="10" max="11" width="21.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="25.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" style="3" customWidth="1"/>
-    <col min="21" max="21" width="19.85546875" style="6" customWidth="1"/>
-    <col min="22" max="22" width="21.42578125" customWidth="1"/>
-    <col min="23" max="23" width="28" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" customWidth="1"/>
-    <col min="25" max="25" width="31.42578125" customWidth="1"/>
-    <col min="26" max="26" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.140625" customWidth="1"/>
-    <col min="29" max="29" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="28" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="27" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="33.7109375" customWidth="1"/>
-    <col min="36" max="36" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="29" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="36.85546875" customWidth="1"/>
-    <col min="60" max="60" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="35" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="38" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="35" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" style="3" customWidth="1"/>
+    <col min="11" max="12" width="21.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="30.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.7109375" style="3" customWidth="1"/>
+    <col min="22" max="22" width="19.85546875" style="6" customWidth="1"/>
+    <col min="23" max="23" width="21.42578125" customWidth="1"/>
+    <col min="24" max="24" width="28" customWidth="1"/>
+    <col min="25" max="25" width="29.28515625" customWidth="1"/>
+    <col min="26" max="26" width="31.42578125" customWidth="1"/>
+    <col min="27" max="27" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="35.140625" customWidth="1"/>
+    <col min="30" max="30" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="27" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="33.7109375" customWidth="1"/>
+    <col min="37" max="37" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="29" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="36.85546875" customWidth="1"/>
+    <col min="61" max="61" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="35" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="38" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="35" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="33" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="19.140625" customWidth="1"/>
+    <col min="81" max="81" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="157.140625" customWidth="1"/>
+    <col min="83" max="83" width="26.5703125" customWidth="1"/>
+    <col min="84" max="84" width="35.28515625" customWidth="1"/>
+    <col min="85" max="85" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>167</v>
       </c>
+      <c r="CB1" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="CF1" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="CG1" s="13" t="s">
+        <v>174</v>
+      </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
-        <v>200</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>70</v>
+      <c r="E2" s="2">
+        <v>200</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="7">
+        <v>70</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="7">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="I2" s="7">
+      <c r="J2" s="7">
         <v>100</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="K2" s="2" t="s">
         <v>94</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="P2" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="R2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V2" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="X2" t="s">
-        <v>25</v>
+      <c r="V2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W2" t="s">
+        <v>24</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="Y2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="7">
+      <c r="AF2" s="7">
         <v>100</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>200</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>70</v>
+      <c r="AH2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>200</v>
       </c>
       <c r="AJ2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AK2" s="7">
+      <c r="AK2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL2" s="7">
         <v>100</v>
-      </c>
-      <c r="AL2" s="10">
-        <v>0</v>
       </c>
       <c r="AM2" s="10">
         <v>0</v>
       </c>
-      <c r="AN2" s="7">
+      <c r="AN2" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="7">
         <v>100</v>
       </c>
-      <c r="AO2" s="7">
+      <c r="AP2" s="7">
         <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="AQ2" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="AR2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AV2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AW2" s="2" t="s">
+      <c r="AW2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AX2" s="2" t="s">
+      <c r="AY2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AY2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>24</v>
-      </c>
-      <c r="BA2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>25</v>
+      <c r="AZ2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BC2" t="s">
-        <v>24</v>
-      </c>
-      <c r="BD2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BE2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BE2" s="2" t="s">
+      <c r="BF2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="BF2" s="2">
-        <v>200</v>
-      </c>
-      <c r="BG2" t="s">
+      <c r="BG2" s="2">
+        <v>200</v>
+      </c>
+      <c r="BH2" t="s">
         <v>37</v>
       </c>
-      <c r="BH2" s="2" t="s">
+      <c r="BI2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BI2" t="s">
-        <v>24</v>
-      </c>
       <c r="BJ2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BK2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BL2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="BL2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>24</v>
+      <c r="BM2" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BN2" t="s">
-        <v>25</v>
-      </c>
-      <c r="BO2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BP2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BP2" t="s">
-        <v>24</v>
-      </c>
-      <c r="BQ2" s="2" t="s">
+      <c r="BQ2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BR2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="BR2" s="2">
-        <v>200</v>
-      </c>
-      <c r="BS2" t="s">
+      <c r="BS2" s="2">
+        <v>200</v>
+      </c>
+      <c r="BT2" t="s">
         <v>37</v>
       </c>
-      <c r="BT2" s="2" t="s">
+      <c r="BU2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BU2" t="s">
-        <v>24</v>
-      </c>
       <c r="BV2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BW2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="BX2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>24</v>
+      <c r="BY2" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BZ2" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>25</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>184</v>
+      </c>
+      <c r="CC2" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CD2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="CE2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="CF2" s="12">
+        <v>200</v>
+      </c>
+      <c r="CG2" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
-        <v>200</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>70</v>
+      <c r="E3" s="2">
+        <v>200</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="7">
+        <v>70</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="7">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I3" s="7">
-        <v>200</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>94</v>
+      <c r="J3" s="7">
+        <v>200</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>94</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="N3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="R3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="S3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V3" t="s">
-        <v>24</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="X3" t="s">
-        <v>25</v>
+      <c r="V3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="Y3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE3" s="7">
-        <v>200</v>
-      </c>
-      <c r="AF3" s="2" t="s">
+      <c r="AF3" s="7">
+        <v>200</v>
+      </c>
+      <c r="AG3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH3" s="2">
-        <v>200</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>70</v>
+      <c r="AH3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>200</v>
       </c>
       <c r="AJ3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AK3" s="7">
-        <v>200</v>
-      </c>
-      <c r="AL3" s="10">
-        <v>0</v>
+      <c r="AK3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL3" s="7">
+        <v>200</v>
       </c>
       <c r="AM3" s="10">
         <v>0</v>
       </c>
-      <c r="AN3" s="7">
-        <v>200</v>
+      <c r="AN3" s="10">
+        <v>0</v>
       </c>
       <c r="AO3" s="7">
+        <v>200</v>
+      </c>
+      <c r="AP3" s="7">
         <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="AP3" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="AQ3" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="AR3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS3" s="3"/>
-      <c r="AT3" s="2" t="s">
+      <c r="AR3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT3" s="3"/>
+      <c r="AU3" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AU3" s="3" t="s">
+      <c r="AV3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AV3" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="AW3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AX3" s="2" t="s">
+      <c r="AY3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="AY3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>24</v>
-      </c>
-      <c r="BA3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>25</v>
+      <c r="AZ3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB3" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BC3" t="s">
-        <v>24</v>
-      </c>
-      <c r="BD3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BE3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BE3" s="2" t="s">
+      <c r="BF3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="BF3" s="2">
-        <v>200</v>
-      </c>
-      <c r="BG3" s="2" t="s">
+      <c r="BG3" s="2">
+        <v>200</v>
+      </c>
+      <c r="BH3" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="BH3" s="2" t="s">
+      <c r="BI3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BI3" t="s">
-        <v>24</v>
-      </c>
       <c r="BJ3" t="s">
-        <v>70</v>
-      </c>
-      <c r="BK3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>70</v>
+      </c>
+      <c r="BL3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BL3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>24</v>
+      <c r="BM3" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BN3" t="s">
-        <v>25</v>
-      </c>
-      <c r="BO3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>25</v>
+      </c>
+      <c r="BP3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BP3" t="s">
-        <v>24</v>
-      </c>
-      <c r="BQ3" s="2" t="s">
+      <c r="BQ3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BR3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BR3" s="2">
-        <v>200</v>
-      </c>
-      <c r="BS3" t="s">
+      <c r="BS3" s="2">
+        <v>200</v>
+      </c>
+      <c r="BT3" t="s">
         <v>111</v>
       </c>
-      <c r="BT3" s="2" t="s">
+      <c r="BU3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BU3" t="s">
-        <v>24</v>
-      </c>
       <c r="BV3" t="s">
-        <v>70</v>
-      </c>
-      <c r="BW3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX3" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BX3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>24</v>
+      <c r="BY3" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BZ3" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>25</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>184</v>
+      </c>
+      <c r="CC3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CD3" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="CE3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="CF3" s="12">
+        <v>200</v>
+      </c>
+      <c r="CG3" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
-        <v>200</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>70</v>
+      <c r="E4" s="2">
+        <v>200</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H4" s="7">
+        <v>70</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="7">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I4" s="7">
+      <c r="J4" s="7">
         <v>300</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="K4" s="2" t="s">
         <v>94</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="P4" s="2" t="s">
+      <c r="N4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="R4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="S4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="U4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V4" t="s">
-        <v>24</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="X4" t="s">
-        <v>25</v>
+      <c r="V4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="Y4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AB4" s="2" t="s">
+      <c r="AC4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AD4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE4" s="7">
+      <c r="AF4" s="7">
         <v>300</v>
       </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AG4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH4" s="2">
-        <v>200</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>70</v>
+      <c r="AH4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>200</v>
       </c>
       <c r="AJ4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AK4" s="7">
+      <c r="AK4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL4" s="7">
         <v>300</v>
-      </c>
-      <c r="AL4" s="10">
-        <v>0</v>
       </c>
       <c r="AM4" s="10">
         <v>0</v>
       </c>
-      <c r="AN4" s="7">
+      <c r="AN4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="7">
         <v>300</v>
       </c>
-      <c r="AO4" s="7">
+      <c r="AP4" s="7">
         <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="AP4" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="AQ4" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="AR4" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS4" s="3"/>
-      <c r="AT4" s="2" t="s">
+      <c r="AR4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT4" s="3"/>
+      <c r="AU4" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AU4" s="3" t="s">
+      <c r="AV4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AV4" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="AW4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AX4" s="2" t="s">
+      <c r="AY4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AY4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>24</v>
-      </c>
-      <c r="BA4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>25</v>
+      <c r="AZ4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB4" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BC4" t="s">
-        <v>24</v>
-      </c>
-      <c r="BD4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BE4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BE4" s="2" t="s">
+      <c r="BF4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="BF4" s="2">
-        <v>200</v>
-      </c>
-      <c r="BG4" s="2" t="s">
+      <c r="BG4" s="2">
+        <v>200</v>
+      </c>
+      <c r="BH4" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="BH4" s="2" t="s">
+      <c r="BI4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BI4" t="s">
-        <v>24</v>
-      </c>
       <c r="BJ4" t="s">
-        <v>70</v>
-      </c>
-      <c r="BK4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BL4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="BL4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BM4" t="s">
-        <v>24</v>
+      <c r="BM4" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BN4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BO4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BP4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BP4" t="s">
-        <v>24</v>
-      </c>
-      <c r="BQ4" s="2" t="s">
+      <c r="BQ4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BR4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="BR4" s="2">
-        <v>200</v>
-      </c>
-      <c r="BS4" t="s">
+      <c r="BS4" s="2">
+        <v>200</v>
+      </c>
+      <c r="BT4" t="s">
         <v>112</v>
       </c>
-      <c r="BT4" s="2" t="s">
+      <c r="BU4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BU4" t="s">
-        <v>24</v>
-      </c>
       <c r="BV4" t="s">
-        <v>70</v>
-      </c>
-      <c r="BW4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BW4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="BX4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BY4" t="s">
-        <v>24</v>
+      <c r="BY4" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BZ4" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>25</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>184</v>
+      </c>
+      <c r="CC4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CD4" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="CE4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="CF4" s="12">
+        <v>200</v>
+      </c>
+      <c r="CG4" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
-        <v>200</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>70</v>
+      <c r="E5" s="2">
+        <v>200</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H5" s="7">
+        <v>70</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="7">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="7">
         <v>400</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="K5" s="2" t="s">
         <v>94</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="P5" s="2" t="s">
+      <c r="N5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q5" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="R5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="U5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="U5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="V5" t="s">
-        <v>24</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="X5" t="s">
-        <v>25</v>
+      <c r="V5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="W5" t="s">
+        <v>24</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="Y5" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA5" s="3" t="s">
+      <c r="AB5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AB5" s="2" t="s">
+      <c r="AC5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AD5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE5" s="7">
+      <c r="AF5" s="7">
         <v>400</v>
       </c>
-      <c r="AF5" s="2" t="s">
+      <c r="AG5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH5" s="2">
-        <v>200</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>70</v>
+      <c r="AH5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>200</v>
       </c>
       <c r="AJ5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AK5" s="7">
+      <c r="AK5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL5" s="7">
         <v>400</v>
-      </c>
-      <c r="AL5" s="10">
-        <v>0</v>
       </c>
       <c r="AM5" s="10">
         <v>0</v>
       </c>
-      <c r="AN5" s="7">
+      <c r="AN5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="7">
         <v>400</v>
       </c>
-      <c r="AO5" s="7">
+      <c r="AP5" s="7">
         <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="AP5" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="AQ5" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="AR5" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS5" s="3"/>
-      <c r="AT5" s="2" t="s">
+      <c r="AR5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AS5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT5" s="3"/>
+      <c r="AU5" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AU5" s="3" t="s">
+      <c r="AV5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AV5" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="AW5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AX5" s="2" t="s">
+      <c r="AY5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AY5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>24</v>
-      </c>
-      <c r="BA5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>25</v>
+      <c r="AZ5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB5" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BC5" t="s">
-        <v>24</v>
-      </c>
-      <c r="BD5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>24</v>
+      </c>
+      <c r="BE5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BE5" s="2" t="s">
+      <c r="BF5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="BF5" s="2">
-        <v>200</v>
-      </c>
-      <c r="BG5" s="2" t="s">
+      <c r="BG5" s="2">
+        <v>200</v>
+      </c>
+      <c r="BH5" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="BH5" s="2" t="s">
+      <c r="BI5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BI5" t="s">
-        <v>24</v>
-      </c>
       <c r="BJ5" t="s">
-        <v>70</v>
-      </c>
-      <c r="BK5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>70</v>
+      </c>
+      <c r="BL5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="BL5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BM5" t="s">
-        <v>24</v>
+      <c r="BM5" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BN5" t="s">
-        <v>25</v>
-      </c>
-      <c r="BO5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BO5" t="s">
+        <v>25</v>
+      </c>
+      <c r="BP5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BP5" t="s">
-        <v>24</v>
-      </c>
-      <c r="BQ5" s="2" t="s">
+      <c r="BQ5" t="s">
+        <v>24</v>
+      </c>
+      <c r="BR5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="BR5" s="2">
-        <v>200</v>
-      </c>
-      <c r="BS5" t="s">
+      <c r="BS5" s="2">
+        <v>200</v>
+      </c>
+      <c r="BT5" t="s">
         <v>113</v>
       </c>
-      <c r="BT5" s="2" t="s">
+      <c r="BU5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="BU5" t="s">
-        <v>24</v>
-      </c>
       <c r="BV5" t="s">
-        <v>70</v>
-      </c>
-      <c r="BW5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BW5" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="BX5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BY5" t="s">
-        <v>24</v>
+      <c r="BY5" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="BZ5" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>25</v>
+      </c>
+      <c r="CB5" t="s">
+        <v>184</v>
+      </c>
+      <c r="CC5" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="CD5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="CE5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="CF5" s="12">
+        <v>200</v>
+      </c>
+      <c r="CG5" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>